<commit_message>
Actualización del entrenamiento del modelo 3, con fotos personales
</commit_message>
<xml_diff>
--- a/facelabels.xlsx
+++ b/facelabels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerar\PycharmProjects\FaceMesh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390C1005-10BC-4624-B16C-BB872C586663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D497671C-F6BA-4643-A549-3C3F06560ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{4304E637-BFEB-48E3-886B-90B278CDA9D1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="8" xr2:uid="{4304E637-BFEB-48E3-886B-90B278CDA9D1}"/>
   </bookViews>
   <sheets>
     <sheet name="divisions" sheetId="1" r:id="rId1"/>
@@ -6587,10 +6587,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33115DCA-41B0-4DF6-BAD8-D4AC1766B5E5}">
-  <dimension ref="A2:A2047"/>
+  <dimension ref="A2:A2056"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2030" workbookViewId="0">
-      <selection activeCell="E2046" sqref="E2046"/>
+    <sheetView topLeftCell="A2030" workbookViewId="0">
+      <selection activeCell="A2048" sqref="A2048:A2056"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16823,6 +16823,51 @@
     <row r="2047" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2047">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2048" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2048">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2049" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2049">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2050" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2050">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2051" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2051">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2052" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2052">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2053" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2053">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2054" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2054">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2055" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2055">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2056" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2056">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -16832,10 +16877,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B7E47E-76FE-41A9-BE75-9035F90BA5A8}">
-  <dimension ref="A2:A2047"/>
+  <dimension ref="A2:A2056"/>
   <sheetViews>
-    <sheetView topLeftCell="A1710" workbookViewId="0">
-      <selection activeCell="G2050" sqref="G2050"/>
+    <sheetView topLeftCell="A2021" workbookViewId="0">
+      <selection activeCell="A2048" sqref="A2048:A2056"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27068,6 +27113,51 @@
     <row r="2047" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2047">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2048" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2048">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2049" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2049">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2050" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2050">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2051" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2051">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2052" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2052">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2053" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2053">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2054" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2054">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2055" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2055">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2056" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2056">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -34547,10 +34637,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D60EF8-B13A-42D8-8DA2-80F2B04406FF}">
-  <dimension ref="A2:A2047"/>
+  <dimension ref="A2:A2056"/>
   <sheetViews>
-    <sheetView topLeftCell="A2012" workbookViewId="0">
-      <selection activeCell="D2021" sqref="D2021"/>
+    <sheetView topLeftCell="A2022" workbookViewId="0">
+      <selection activeCell="A2048" sqref="A2048:A2056"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -44783,6 +44873,51 @@
     <row r="2047" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2047">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2048" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2048">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2049" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2049">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2050" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2050">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2051" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2051">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2052" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2052">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2053" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2053">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2054" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2054">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2055" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2055">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2056" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2056">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -48527,10 +48662,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1152A14B-003E-488A-9976-96BC184DC5F4}">
-  <dimension ref="A2:A2047"/>
+  <dimension ref="A2:A2056"/>
   <sheetViews>
-    <sheetView topLeftCell="A2011" workbookViewId="0">
-      <selection activeCell="G2026" sqref="G2026"/>
+    <sheetView tabSelected="1" topLeftCell="A2019" workbookViewId="0">
+      <selection activeCell="P2047" sqref="P2047"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -58765,6 +58900,51 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2048" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2048">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2049" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2049">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2050" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2050">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2051" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2051">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2052" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2052">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2053" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2053">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2054" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2054">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2055" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2055">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2056" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2056">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrega código para imagenes de perdida y exactitud de los modelos
</commit_message>
<xml_diff>
--- a/facelabels.xlsx
+++ b/facelabels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerar\PycharmProjects\FaceMesh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D497671C-F6BA-4643-A549-3C3F06560ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7021D4-4123-49CC-A645-0E150F436DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="8" xr2:uid="{4304E637-BFEB-48E3-886B-90B278CDA9D1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{4304E637-BFEB-48E3-886B-90B278CDA9D1}"/>
   </bookViews>
   <sheets>
     <sheet name="divisions" sheetId="1" r:id="rId1"/>
@@ -462,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F696E24-BC24-4B71-82B1-F1705421A9EC}">
-  <dimension ref="A1:AE59"/>
+  <dimension ref="A1:AE64"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2:AE16"/>
+    <sheetView tabSelected="1" topLeftCell="H32" workbookViewId="0">
+      <selection activeCell="Y64" sqref="Y64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2512,7 +2512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="18:30" x14ac:dyDescent="0.35">
+    <row r="49" spans="17:30" x14ac:dyDescent="0.35">
       <c r="R49">
         <v>0</v>
       </c>
@@ -2553,12 +2553,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="18:30" x14ac:dyDescent="0.35">
+    <row r="51" spans="17:30" x14ac:dyDescent="0.35">
       <c r="R51" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="18:30" x14ac:dyDescent="0.35">
+    <row r="53" spans="17:30" x14ac:dyDescent="0.35">
       <c r="R53">
         <v>3</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="18:30" x14ac:dyDescent="0.35">
+    <row r="54" spans="17:30" x14ac:dyDescent="0.35">
       <c r="R54">
         <v>3</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="18:30" x14ac:dyDescent="0.35">
+    <row r="55" spans="17:30" x14ac:dyDescent="0.35">
       <c r="R55">
         <v>3</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="18:30" x14ac:dyDescent="0.35">
+    <row r="56" spans="17:30" x14ac:dyDescent="0.35">
       <c r="R56">
         <v>0</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="18:30" x14ac:dyDescent="0.35">
+    <row r="57" spans="17:30" x14ac:dyDescent="0.35">
       <c r="R57">
         <v>0</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="18:30" x14ac:dyDescent="0.35">
+    <row r="58" spans="17:30" x14ac:dyDescent="0.35">
       <c r="R58">
         <v>0</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="18:30" x14ac:dyDescent="0.35">
+    <row r="59" spans="17:30" x14ac:dyDescent="0.35">
       <c r="R59">
         <v>0</v>
       </c>
@@ -2843,6 +2843,16 @@
       </c>
       <c r="AD59">
         <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="17:30" x14ac:dyDescent="0.35">
+      <c r="Q63">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="17:30" x14ac:dyDescent="0.35">
+      <c r="Q64">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -6587,10 +6597,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33115DCA-41B0-4DF6-BAD8-D4AC1766B5E5}">
-  <dimension ref="A2:A2056"/>
+  <dimension ref="A2:A2069"/>
   <sheetViews>
-    <sheetView topLeftCell="A2030" workbookViewId="0">
-      <selection activeCell="A2048" sqref="A2048:A2056"/>
+    <sheetView topLeftCell="A2039" workbookViewId="0">
+      <selection activeCell="A2048" sqref="A2048:A2069"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16837,36 +16847,101 @@
     </row>
     <row r="2050" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2050">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2051" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2051">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2052" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2052">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2053" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2053">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2054" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2054">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2055" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2055">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2056" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2056">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2057" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2057">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2058" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2058">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2059" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2059">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2060" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2060">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2061" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2061">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2062" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2062">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2063" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2063">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2064" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2064">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2065" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2065">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2066" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2066">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2067" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2067">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2068" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2068">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2069" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2069">
         <v>5</v>
       </c>
     </row>
@@ -16877,10 +16952,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B7E47E-76FE-41A9-BE75-9035F90BA5A8}">
-  <dimension ref="A2:A2056"/>
+  <dimension ref="A2:A2069"/>
   <sheetViews>
-    <sheetView topLeftCell="A2021" workbookViewId="0">
-      <selection activeCell="A2048" sqref="A2048:A2056"/>
+    <sheetView topLeftCell="A2029" workbookViewId="0">
+      <selection activeCell="A2048" sqref="A2048:A2069"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27127,36 +27202,101 @@
     </row>
     <row r="2050" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2050">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2051" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2051">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2052" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2052">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2053" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2053">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2054" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2054">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2055" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2055">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2056" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2056">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2057" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2057">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2058" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2058">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2059" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2059">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2060" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2060">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2061" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2061">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2062" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2062">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2063" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2063">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2064" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2064">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2065" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2065">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2066" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2066">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2067" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2067">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2068" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2068">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2069" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2069">
         <v>5</v>
       </c>
     </row>
@@ -34637,10 +34777,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D60EF8-B13A-42D8-8DA2-80F2B04406FF}">
-  <dimension ref="A2:A2056"/>
+  <dimension ref="A2:A2069"/>
   <sheetViews>
-    <sheetView topLeftCell="A2022" workbookViewId="0">
-      <selection activeCell="A2048" sqref="A2048:A2056"/>
+    <sheetView topLeftCell="A2027" workbookViewId="0">
+      <selection activeCell="A2048" sqref="A2048:A2069"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -44887,36 +45027,101 @@
     </row>
     <row r="2050" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2050">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2051" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2051">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2052" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2052">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2053" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2053">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2054" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2054">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2055" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2055">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2056" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2056">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2057" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2057">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2058" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2058">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2059" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2059">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2060" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2060">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2061" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2061">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2062" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2062">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2063" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2063">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2064" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2064">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2065" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2065">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2066" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2066">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2067" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2067">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2068" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2068">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2069" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2069">
         <v>5</v>
       </c>
     </row>
@@ -48662,10 +48867,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1152A14B-003E-488A-9976-96BC184DC5F4}">
-  <dimension ref="A2:A2056"/>
+  <dimension ref="A2:A2069"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2019" workbookViewId="0">
-      <selection activeCell="P2047" sqref="P2047"/>
+    <sheetView topLeftCell="A2028" workbookViewId="0">
+      <selection activeCell="P2042" sqref="P2042"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -58912,36 +59117,101 @@
     </row>
     <row r="2050" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2050">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2051" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2051">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2052" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2052">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2053" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2053">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2054" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2054">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2055" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2055">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2056" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2056">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2057" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2057">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2058" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2058">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2059" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2059">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2060" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2060">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2061" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2061">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2062" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2062">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2063" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2063">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2064" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2064">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2065" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2065">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2066" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2066">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2067" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2067">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2068" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2068">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2069" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2069">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se ordenaron los codigos para poder interactuar de una maner más cómoda
</commit_message>
<xml_diff>
--- a/facelabels.xlsx
+++ b/facelabels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerar\PycharmProjects\FaceMesh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5F0CDE-8A20-4B56-B869-B61922A99870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A6E133-9A01-4016-9995-BCC7A6136F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{4304E637-BFEB-48E3-886B-90B278CDA9D1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="8" xr2:uid="{4304E637-BFEB-48E3-886B-90B278CDA9D1}"/>
   </bookViews>
   <sheets>
     <sheet name="divisions" sheetId="1" r:id="rId1"/>
@@ -13219,7 +13219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D60EF8-B13A-42D8-8DA2-80F2B04406FF}">
   <dimension ref="A2:A2069"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2039" workbookViewId="0">
+    <sheetView topLeftCell="A2039" workbookViewId="0">
       <selection activeCell="F2055" sqref="F2055"/>
     </sheetView>
   </sheetViews>
@@ -55489,7 +55489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4134E259-5FCC-4104-B38D-C89F68DE518F}">
   <dimension ref="A2:A745"/>
   <sheetViews>
-    <sheetView topLeftCell="A718" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A718" workbookViewId="0">
       <selection activeCell="H749" sqref="H749"/>
     </sheetView>
   </sheetViews>

</xml_diff>